<commit_message>
fixed some bugs in data (max size of roach and bream), finished exploring data on consumption and metabolism
</commit_message>
<xml_diff>
--- a/data/consumption_scaling_data.xlsx
+++ b/data/consumption_scaling_data.xlsx
@@ -2484,9 +2484,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z104" sqref="Z104"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O37" sqref="O37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4006,7 +4006,7 @@
         <v>72</v>
       </c>
       <c r="Q20" s="4">
-        <v>6000</v>
+        <v>1800</v>
       </c>
       <c r="R20" s="4">
         <v>10</v>
@@ -4084,7 +4084,7 @@
         <v>72</v>
       </c>
       <c r="Q21" s="4">
-        <v>6000</v>
+        <v>1800</v>
       </c>
       <c r="R21" s="4">
         <v>10</v>
@@ -4162,7 +4162,7 @@
         <v>72</v>
       </c>
       <c r="Q22" s="4">
-        <v>6000</v>
+        <v>1800</v>
       </c>
       <c r="R22" s="4">
         <v>10</v>
@@ -4240,7 +4240,7 @@
         <v>72</v>
       </c>
       <c r="Q23" s="4">
-        <v>6000</v>
+        <v>1800</v>
       </c>
       <c r="R23" s="4">
         <v>10</v>

</xml_diff>

<commit_message>
- update analysis (random intercept only) - multiple regression for rates - new figures
</commit_message>
<xml_diff>
--- a/data/consumption_scaling_data.xlsx
+++ b/data/consumption_scaling_data.xlsx
@@ -1136,9 +1136,6 @@
     <t>reef-associated; oceanodromous</t>
   </si>
   <si>
-    <t>Western Mosquitofish</t>
-  </si>
-  <si>
     <t>Gambusia affinis</t>
   </si>
   <si>
@@ -2100,6 +2097,9 @@
   </si>
   <si>
     <t>313.935806071488</t>
+  </si>
+  <si>
+    <t>Western mosquitofish</t>
   </si>
 </sst>
 </file>
@@ -2484,9 +2484,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O37" sqref="O37"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H80" sqref="H80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2530,16 +2530,16 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>581</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>582</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>583</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>5</v>
@@ -2560,34 +2560,34 @@
         <v>11</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>584</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>585</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>152</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>610</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>611</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>612</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>613</v>
       </c>
-      <c r="U1" s="1" t="s">
-        <v>614</v>
-      </c>
       <c r="V1" s="1" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="Y1" s="6" t="s">
         <v>349</v>
@@ -2596,24 +2596,24 @@
         <v>6</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="2" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>604</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>603</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>605</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>604</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>606</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>607</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>608</v>
       </c>
       <c r="F2" s="4">
         <v>16</v>
@@ -2661,10 +2661,10 @@
         <v>5</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="W2" s="11" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="X2" s="4" t="s">
         <v>10</v>
@@ -2673,10 +2673,10 @@
         <v>351</v>
       </c>
       <c r="Z2" s="4" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="AA2" s="4" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="3" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -2735,10 +2735,10 @@
         <v>352</v>
       </c>
       <c r="U3" s="4" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="W3" s="4" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="X3" s="4" t="s">
         <v>21</v>
@@ -2810,7 +2810,7 @@
       </c>
       <c r="V4" s="4"/>
       <c r="W4" s="4" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="X4" s="4" t="s">
         <v>21</v>
@@ -2819,10 +2819,10 @@
         <v>351</v>
       </c>
       <c r="Z4" s="5" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="AA4" s="5" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="5" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2881,11 +2881,11 @@
         <v>238</v>
       </c>
       <c r="U5" s="4" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="V5" s="4"/>
       <c r="W5" s="4" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="X5" s="4" t="s">
         <v>21</v>
@@ -2897,7 +2897,7 @@
         <v>218</v>
       </c>
       <c r="AA5" s="5" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="6" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -2959,7 +2959,7 @@
         <v>64</v>
       </c>
       <c r="W6" s="4" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="X6" s="4" t="s">
         <v>21</v>
@@ -3027,10 +3027,10 @@
         <v>20</v>
       </c>
       <c r="U7" s="4" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="W7" s="7" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="X7" s="4" t="s">
         <v>21</v>
@@ -3039,7 +3039,7 @@
         <v>351</v>
       </c>
       <c r="Z7" s="4" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="AA7" s="4" t="s">
         <v>278</v>
@@ -3101,10 +3101,10 @@
         <v>296</v>
       </c>
       <c r="U8" s="4" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="W8" s="4" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="X8" s="4" t="s">
         <v>21</v>
@@ -3113,7 +3113,7 @@
         <v>351</v>
       </c>
       <c r="Z8" s="4" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="AA8" s="4" t="s">
         <v>297</v>
@@ -3178,7 +3178,7 @@
         <v>64</v>
       </c>
       <c r="W9" s="4" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="X9" s="4" t="s">
         <v>21</v>
@@ -3213,7 +3213,7 @@
         <v>314</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>315</v>
@@ -3252,10 +3252,10 @@
         <v>3</v>
       </c>
       <c r="U10" s="4" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="W10" s="7" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="X10" s="4" t="s">
         <v>10</v>
@@ -3272,7 +3272,7 @@
         <v>189</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E11" s="4">
         <v>25</v>
@@ -3281,13 +3281,13 @@
         <v>72</v>
       </c>
       <c r="G11" s="4" t="s">
+        <v>449</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>450</v>
       </c>
-      <c r="H11" s="4" t="s">
-        <v>451</v>
-      </c>
       <c r="I11" s="4" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>260</v>
@@ -3308,7 +3308,7 @@
         <v>307</v>
       </c>
       <c r="P11" s="4" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="Q11" s="4">
         <v>3000</v>
@@ -3326,7 +3326,7 @@
         <v>64</v>
       </c>
       <c r="W11" s="4" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="X11" s="4" t="s">
         <v>21</v>
@@ -3336,15 +3336,15 @@
       </c>
       <c r="Z11" s="9"/>
       <c r="AA11" s="4" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="12" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
+        <v>452</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>453</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>454</v>
       </c>
       <c r="E12" s="4">
         <v>30</v>
@@ -3356,16 +3356,16 @@
         <v>129</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="I12" s="4" t="s">
+        <v>455</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>454</v>
+      </c>
+      <c r="K12" s="4" t="s">
         <v>456</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>455</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>457</v>
       </c>
       <c r="L12" s="4" t="s">
         <v>19</v>
@@ -3380,7 +3380,7 @@
         <v>62</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="Q12" s="4">
         <v>2700</v>
@@ -3398,7 +3398,7 @@
         <v>64</v>
       </c>
       <c r="W12" s="4" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="X12" s="4" t="s">
         <v>21</v>
@@ -3408,36 +3408,36 @@
       </c>
       <c r="Z12" s="9"/>
       <c r="AA12" s="4" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="13" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>461</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>462</v>
       </c>
       <c r="E13" s="4">
         <v>20</v>
       </c>
       <c r="F13" s="8" t="s">
+        <v>462</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>463</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="H13" s="4" t="s">
+        <v>459</v>
+      </c>
+      <c r="I13" s="4" t="s">
         <v>464</v>
       </c>
-      <c r="H13" s="4" t="s">
-        <v>460</v>
-      </c>
-      <c r="I13" s="4" t="s">
+      <c r="J13" s="4" t="s">
         <v>465</v>
       </c>
-      <c r="J13" s="4" t="s">
+      <c r="K13" s="4" t="s">
         <v>466</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>467</v>
       </c>
       <c r="L13" s="4" t="s">
         <v>60</v>
@@ -3470,7 +3470,7 @@
         <v>64</v>
       </c>
       <c r="W13" s="4" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="X13" s="4" t="s">
         <v>21</v>
@@ -3479,39 +3479,39 @@
         <v>351</v>
       </c>
       <c r="Z13" s="4" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="AA13" s="4" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="14" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
+        <v>492</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>491</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>493</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>492</v>
-      </c>
-      <c r="C14" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>494</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>495</v>
       </c>
       <c r="E14" s="4">
         <v>10</v>
       </c>
       <c r="F14" s="8" t="s">
+        <v>495</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>496</v>
       </c>
-      <c r="G14" s="4" t="s">
-        <v>497</v>
-      </c>
       <c r="H14" s="4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>213</v>
@@ -3520,7 +3520,7 @@
         <v>36</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="M14" s="4" t="s">
         <v>357</v>
@@ -3532,7 +3532,7 @@
         <v>12</v>
       </c>
       <c r="P14" s="4" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="Q14" s="4">
         <v>14500</v>
@@ -3550,7 +3550,7 @@
         <v>64</v>
       </c>
       <c r="W14" s="7" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="X14" s="4" t="s">
         <v>10</v>
@@ -3559,39 +3559,39 @@
         <v>351</v>
       </c>
       <c r="Z14" s="9" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="AA14" s="4" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="15" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
+        <v>525</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>523</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>526</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>524</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>527</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>525</v>
       </c>
       <c r="E15" s="4">
         <v>8</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="J15" s="4" t="s">
         <v>169</v>
@@ -3606,7 +3606,7 @@
         <v>356</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="O15" s="4" t="s">
         <v>12</v>
@@ -3627,10 +3627,10 @@
         <v>9</v>
       </c>
       <c r="U15" s="4" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="W15" s="4" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="X15" s="4" t="s">
         <v>10</v>
@@ -3639,10 +3639,10 @@
         <v>351</v>
       </c>
       <c r="Z15" s="7" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="AA15" s="4" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="16" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -3710,7 +3710,7 @@
         <v>64</v>
       </c>
       <c r="W16" s="4" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="X16" s="4" t="s">
         <v>21</v>
@@ -3788,7 +3788,7 @@
       </c>
       <c r="V17" s="3"/>
       <c r="W17" s="4" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="X17" s="3" t="s">
         <v>21</v>
@@ -3866,7 +3866,7 @@
       </c>
       <c r="V18" s="3"/>
       <c r="W18" s="4" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="X18" s="3" t="s">
         <v>21</v>
@@ -3944,7 +3944,7 @@
       </c>
       <c r="V19" s="3"/>
       <c r="W19" s="4" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="X19" s="3" t="s">
         <v>21</v>
@@ -4022,7 +4022,7 @@
       </c>
       <c r="V20" s="3"/>
       <c r="W20" s="4" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="X20" s="3" t="s">
         <v>21</v>
@@ -4100,7 +4100,7 @@
       </c>
       <c r="V21" s="3"/>
       <c r="W21" s="4" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="X21" s="3" t="s">
         <v>21</v>
@@ -4178,7 +4178,7 @@
       </c>
       <c r="V22" s="3"/>
       <c r="W22" s="4" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="X22" s="3" t="s">
         <v>21</v>
@@ -4256,7 +4256,7 @@
       </c>
       <c r="V23" s="3"/>
       <c r="W23" s="4" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="X23" s="3" t="s">
         <v>21</v>
@@ -4327,7 +4327,7 @@
         <v>64</v>
       </c>
       <c r="W24" s="3" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="X24" s="3" t="s">
         <v>21</v>
@@ -4398,7 +4398,7 @@
         <v>64</v>
       </c>
       <c r="W25" s="3" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="X25" s="3" t="s">
         <v>21</v>
@@ -4469,7 +4469,7 @@
         <v>64</v>
       </c>
       <c r="W26" s="3" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="X26" s="3" t="s">
         <v>21</v>
@@ -4540,7 +4540,7 @@
         <v>64</v>
       </c>
       <c r="W27" s="3" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="X27" s="3" t="s">
         <v>21</v>
@@ -4611,7 +4611,7 @@
         <v>64</v>
       </c>
       <c r="W28" s="3" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="X28" s="3" t="s">
         <v>21</v>
@@ -4643,7 +4643,7 @@
         <v>281</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="I29" s="3" t="s">
         <v>34</v>
@@ -4682,10 +4682,10 @@
         <v>238</v>
       </c>
       <c r="U29" s="4" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="W29" s="3" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="X29" s="3" t="s">
         <v>21</v>
@@ -4694,10 +4694,10 @@
         <v>351</v>
       </c>
       <c r="Z29" s="3" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="AA29" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="30" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -4720,7 +4720,7 @@
         <v>281</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="I30" s="3" t="s">
         <v>34</v>
@@ -4759,10 +4759,10 @@
         <v>238</v>
       </c>
       <c r="U30" s="4" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="W30" s="3" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="X30" s="3" t="s">
         <v>21</v>
@@ -4771,7 +4771,7 @@
         <v>351</v>
       </c>
       <c r="Z30" s="3" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="AA30" s="3" t="s">
         <v>54</v>
@@ -4797,7 +4797,7 @@
         <v>281</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="I31" s="3" t="s">
         <v>34</v>
@@ -4836,10 +4836,10 @@
         <v>238</v>
       </c>
       <c r="U31" s="4" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="W31" s="3" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="X31" s="3" t="s">
         <v>21</v>
@@ -4848,7 +4848,7 @@
         <v>351</v>
       </c>
       <c r="Z31" s="3" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="AA31" s="3" t="s">
         <v>54</v>
@@ -4874,7 +4874,7 @@
         <v>281</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="I32" s="3" t="s">
         <v>34</v>
@@ -4913,10 +4913,10 @@
         <v>238</v>
       </c>
       <c r="U32" s="4" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="W32" s="3" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="X32" s="3" t="s">
         <v>21</v>
@@ -4925,7 +4925,7 @@
         <v>351</v>
       </c>
       <c r="Z32" s="3" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="AA32" s="3" t="s">
         <v>54</v>
@@ -4987,11 +4987,11 @@
         <v>13</v>
       </c>
       <c r="U33" s="4" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="V33" s="3"/>
       <c r="W33" s="4" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="X33" s="4" t="s">
         <v>10</v>
@@ -5061,10 +5061,10 @@
         <v>13</v>
       </c>
       <c r="U34" s="4" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="W34" s="4" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="X34" s="4" t="s">
         <v>10</v>
@@ -5135,10 +5135,10 @@
         <v>13</v>
       </c>
       <c r="U35" s="4" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="W35" s="4" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="X35" s="4" t="s">
         <v>10</v>
@@ -5209,10 +5209,10 @@
         <v>13</v>
       </c>
       <c r="U36" s="4" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="W36" s="4" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="X36" s="4" t="s">
         <v>10</v>
@@ -5283,10 +5283,10 @@
         <v>13</v>
       </c>
       <c r="U37" s="4" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="W37" s="4" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="X37" s="4" t="s">
         <v>10</v>
@@ -5357,10 +5357,10 @@
         <v>276</v>
       </c>
       <c r="U38" s="4" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="W38" s="11" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="X38" s="4" t="s">
         <v>21</v>
@@ -5429,10 +5429,10 @@
         <v>276</v>
       </c>
       <c r="U39" s="4" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="W39" s="11" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="X39" s="4" t="s">
         <v>21</v>
@@ -5500,10 +5500,10 @@
         <v>276</v>
       </c>
       <c r="U40" s="4" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="W40" s="11" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="X40" s="4" t="s">
         <v>21</v>
@@ -5571,10 +5571,10 @@
         <v>276</v>
       </c>
       <c r="U41" s="4" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="W41" s="11" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="X41" s="4" t="s">
         <v>21</v>
@@ -5642,10 +5642,10 @@
         <v>276</v>
       </c>
       <c r="U42" s="4" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="W42" s="11" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="X42" s="4" t="s">
         <v>21</v>
@@ -5713,10 +5713,10 @@
         <v>276</v>
       </c>
       <c r="U43" s="4" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="W43" s="11" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="X43" s="4" t="s">
         <v>21</v>
@@ -5784,10 +5784,10 @@
         <v>15</v>
       </c>
       <c r="U44" s="4" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="W44" s="11" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="X44" s="4" t="s">
         <v>21</v>
@@ -5855,10 +5855,10 @@
         <v>15</v>
       </c>
       <c r="U45" s="4" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="W45" s="11" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="X45" s="4" t="s">
         <v>21</v>
@@ -5926,10 +5926,10 @@
         <v>15</v>
       </c>
       <c r="U46" s="4" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="W46" s="11" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="X46" s="4" t="s">
         <v>21</v>
@@ -5997,10 +5997,10 @@
         <v>15</v>
       </c>
       <c r="U47" s="4" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="W47" s="11" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="X47" s="4" t="s">
         <v>21</v>
@@ -6068,10 +6068,10 @@
         <v>15</v>
       </c>
       <c r="U48" s="4" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="W48" s="11" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="X48" s="4" t="s">
         <v>21</v>
@@ -6139,10 +6139,10 @@
         <v>15</v>
       </c>
       <c r="U49" s="4" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="W49" s="11" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="X49" s="4" t="s">
         <v>21</v>
@@ -6213,7 +6213,7 @@
         <v>64</v>
       </c>
       <c r="W50" s="7" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="X50" s="3" t="s">
         <v>10</v>
@@ -6284,7 +6284,7 @@
         <v>64</v>
       </c>
       <c r="W51" s="7" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="X51" s="3" t="s">
         <v>10</v>
@@ -6355,7 +6355,7 @@
         <v>64</v>
       </c>
       <c r="W52" s="13" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="X52" s="3" t="s">
         <v>10</v>
@@ -6426,7 +6426,7 @@
         <v>64</v>
       </c>
       <c r="W53" s="13" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="X53" s="3" t="s">
         <v>10</v>
@@ -6443,7 +6443,7 @@
         <v>130</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E54" s="4">
         <v>35</v>
@@ -6494,10 +6494,10 @@
         <v>277</v>
       </c>
       <c r="U54" s="4" t="s">
+        <v>624</v>
+      </c>
+      <c r="W54" s="11" t="s">
         <v>625</v>
-      </c>
-      <c r="W54" s="11" t="s">
-        <v>626</v>
       </c>
       <c r="X54" s="4" t="s">
         <v>21</v>
@@ -6515,7 +6515,7 @@
         <v>131</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E55" s="4">
         <v>33</v>
@@ -6566,10 +6566,10 @@
         <v>277</v>
       </c>
       <c r="U55" s="4" t="s">
+        <v>624</v>
+      </c>
+      <c r="W55" s="11" t="s">
         <v>625</v>
-      </c>
-      <c r="W55" s="11" t="s">
-        <v>626</v>
       </c>
       <c r="X55" s="4" t="s">
         <v>21</v>
@@ -6586,7 +6586,7 @@
         <v>132</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="E56" s="4">
         <v>31</v>
@@ -6637,10 +6637,10 @@
         <v>277</v>
       </c>
       <c r="U56" s="4" t="s">
+        <v>624</v>
+      </c>
+      <c r="W56" s="11" t="s">
         <v>625</v>
-      </c>
-      <c r="W56" s="11" t="s">
-        <v>626</v>
       </c>
       <c r="X56" s="4" t="s">
         <v>21</v>
@@ -6657,7 +6657,7 @@
         <v>133</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="E57" s="4">
         <v>27</v>
@@ -6708,10 +6708,10 @@
         <v>277</v>
       </c>
       <c r="U57" s="4" t="s">
+        <v>624</v>
+      </c>
+      <c r="W57" s="11" t="s">
         <v>625</v>
-      </c>
-      <c r="W57" s="11" t="s">
-        <v>626</v>
       </c>
       <c r="X57" s="4" t="s">
         <v>21</v>
@@ -6728,7 +6728,7 @@
         <v>116</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="E58" s="4">
         <v>23</v>
@@ -6779,10 +6779,10 @@
         <v>277</v>
       </c>
       <c r="U58" s="4" t="s">
+        <v>624</v>
+      </c>
+      <c r="W58" s="11" t="s">
         <v>625</v>
-      </c>
-      <c r="W58" s="11" t="s">
-        <v>626</v>
       </c>
       <c r="X58" s="4" t="s">
         <v>21</v>
@@ -6853,7 +6853,7 @@
         <v>64</v>
       </c>
       <c r="W59" s="11" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="X59" s="4" t="s">
         <v>10</v>
@@ -6862,7 +6862,7 @@
         <v>351</v>
       </c>
       <c r="Z59" s="4" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="AA59" s="4" t="s">
         <v>162</v>
@@ -6927,7 +6927,7 @@
         <v>64</v>
       </c>
       <c r="W60" s="11" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="X60" s="4" t="s">
         <v>10</v>
@@ -6936,7 +6936,7 @@
         <v>351</v>
       </c>
       <c r="Z60" s="4" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="AA60" s="4" t="s">
         <v>162</v>
@@ -7001,7 +7001,7 @@
         <v>64</v>
       </c>
       <c r="W61" s="11" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="X61" s="4" t="s">
         <v>10</v>
@@ -7010,7 +7010,7 @@
         <v>351</v>
       </c>
       <c r="Z61" s="4" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="AA61" s="4" t="s">
         <v>162</v>
@@ -7075,7 +7075,7 @@
         <v>64</v>
       </c>
       <c r="W62" s="4" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="X62" s="4" t="s">
         <v>10</v>
@@ -7084,7 +7084,7 @@
         <v>351</v>
       </c>
       <c r="Z62" s="4" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="AA62" s="4" t="s">
         <v>162</v>
@@ -7155,7 +7155,7 @@
         <v>8</v>
       </c>
       <c r="W63" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="X63" s="3" t="s">
         <v>21</v>
@@ -7232,7 +7232,7 @@
         <v>8</v>
       </c>
       <c r="W64" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="X64" s="3" t="s">
         <v>21</v>
@@ -7309,7 +7309,7 @@
         <v>8</v>
       </c>
       <c r="W65" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="X65" s="3" t="s">
         <v>21</v>
@@ -7380,7 +7380,7 @@
         <v>64</v>
       </c>
       <c r="W66" s="7" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="X66" s="3" t="s">
         <v>21</v>
@@ -7451,7 +7451,7 @@
         <v>64</v>
       </c>
       <c r="W67" s="7" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="X67" s="3" t="s">
         <v>21</v>
@@ -7522,7 +7522,7 @@
         <v>64</v>
       </c>
       <c r="W68" s="7" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="X68" s="3" t="s">
         <v>21</v>
@@ -7593,7 +7593,7 @@
         <v>64</v>
       </c>
       <c r="W69" s="7" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="X69" s="3" t="s">
         <v>21</v>
@@ -7664,7 +7664,7 @@
         <v>64</v>
       </c>
       <c r="W70" s="7" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="X70" s="3" t="s">
         <v>21</v>
@@ -7735,7 +7735,7 @@
         <v>64</v>
       </c>
       <c r="W71" s="7" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="X71" s="3" t="s">
         <v>21</v>
@@ -7806,7 +7806,7 @@
         <v>64</v>
       </c>
       <c r="W72" s="7" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="X72" s="4" t="s">
         <v>21</v>
@@ -7877,7 +7877,7 @@
         <v>64</v>
       </c>
       <c r="W73" s="7" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="X73" s="4" t="s">
         <v>21</v>
@@ -7948,7 +7948,7 @@
         <v>64</v>
       </c>
       <c r="W74" s="7" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="X74" s="4" t="s">
         <v>21</v>
@@ -8019,7 +8019,7 @@
         <v>64</v>
       </c>
       <c r="W75" s="7" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="X75" s="3" t="s">
         <v>21</v>
@@ -8090,7 +8090,7 @@
         <v>64</v>
       </c>
       <c r="W76" s="7" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="X76" s="3" t="s">
         <v>21</v>
@@ -8161,7 +8161,7 @@
         <v>64</v>
       </c>
       <c r="W77" s="7" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="X77" s="3" t="s">
         <v>21</v>
@@ -8233,7 +8233,7 @@
       </c>
       <c r="V78" s="4"/>
       <c r="W78" s="7" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="X78" s="5" t="s">
         <v>10</v>
@@ -8242,10 +8242,10 @@
         <v>350</v>
       </c>
       <c r="Z78" s="4" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="AA78" s="5" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="79" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -8308,7 +8308,7 @@
       </c>
       <c r="V79" s="4"/>
       <c r="W79" s="7" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="X79" s="5" t="s">
         <v>10</v>
@@ -8317,10 +8317,10 @@
         <v>350</v>
       </c>
       <c r="Z79" s="4" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="AA79" s="5" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="80" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -8383,7 +8383,7 @@
       </c>
       <c r="V80" s="4"/>
       <c r="W80" s="7" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="X80" s="5" t="s">
         <v>10</v>
@@ -8392,10 +8392,10 @@
         <v>351</v>
       </c>
       <c r="Z80" s="4" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="AA80" s="5" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="81" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -8458,7 +8458,7 @@
       </c>
       <c r="V81" s="4"/>
       <c r="W81" s="7" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="X81" s="5" t="s">
         <v>10</v>
@@ -8467,48 +8467,48 @@
         <v>350</v>
       </c>
       <c r="Z81" s="4" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="AA81" s="5" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="82" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="C82" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="B82" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>382</v>
-      </c>
       <c r="D82" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E82" s="2">
         <v>5</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H82" s="2" t="s">
+        <v>691</v>
+      </c>
+      <c r="I82" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="I82" s="2" t="s">
+      <c r="J82" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="J82" s="2" t="s">
+      <c r="K82" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="K82" s="2" t="s">
+      <c r="L82" s="2" t="s">
         <v>373</v>
-      </c>
-      <c r="L82" s="2" t="s">
-        <v>374</v>
       </c>
       <c r="M82" s="4" t="s">
         <v>357</v>
@@ -8523,7 +8523,7 @@
         <v>174</v>
       </c>
       <c r="Q82" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="R82" s="2">
         <v>12</v>
@@ -8538,7 +8538,7 @@
         <v>64</v>
       </c>
       <c r="W82" s="7" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="X82" s="5" t="s">
         <v>10</v>
@@ -8547,45 +8547,45 @@
         <v>351</v>
       </c>
       <c r="AA82" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="83" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="C83" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="B83" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="C83" s="2" t="s">
+      <c r="D83" s="2" t="s">
         <v>385</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>386</v>
       </c>
       <c r="E83" s="2">
         <v>15</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="H83" s="2" t="s">
+        <v>691</v>
+      </c>
+      <c r="I83" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="I83" s="2" t="s">
+      <c r="J83" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="J83" s="2" t="s">
+      <c r="K83" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="K83" s="2" t="s">
+      <c r="L83" s="2" t="s">
         <v>373</v>
-      </c>
-      <c r="L83" s="2" t="s">
-        <v>374</v>
       </c>
       <c r="M83" s="4" t="s">
         <v>357</v>
@@ -8600,7 +8600,7 @@
         <v>174</v>
       </c>
       <c r="Q83" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="R83" s="2">
         <v>12</v>
@@ -8615,7 +8615,7 @@
         <v>64</v>
       </c>
       <c r="W83" s="7" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="X83" s="5" t="s">
         <v>10</v>
@@ -8624,45 +8624,45 @@
         <v>351</v>
       </c>
       <c r="AA83" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="84" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="C84" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="B84" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="C84" s="2" t="s">
+      <c r="D84" s="2" t="s">
         <v>390</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>391</v>
       </c>
       <c r="E84" s="2">
         <v>25</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="H84" s="2" t="s">
+        <v>691</v>
+      </c>
+      <c r="I84" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="I84" s="2" t="s">
+      <c r="J84" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="J84" s="2" t="s">
+      <c r="K84" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="K84" s="2" t="s">
+      <c r="L84" s="2" t="s">
         <v>373</v>
-      </c>
-      <c r="L84" s="2" t="s">
-        <v>374</v>
       </c>
       <c r="M84" s="4" t="s">
         <v>357</v>
@@ -8677,7 +8677,7 @@
         <v>174</v>
       </c>
       <c r="Q84" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="R84" s="2">
         <v>12</v>
@@ -8692,7 +8692,7 @@
         <v>64</v>
       </c>
       <c r="W84" s="7" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="X84" s="5" t="s">
         <v>10</v>
@@ -8701,45 +8701,45 @@
         <v>351</v>
       </c>
       <c r="AA84" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="85" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="C85" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="B85" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="C85" s="2" t="s">
+      <c r="D85" s="2" t="s">
         <v>396</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>397</v>
       </c>
       <c r="E85" s="2">
         <v>32</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="H85" s="2" t="s">
+        <v>691</v>
+      </c>
+      <c r="I85" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="I85" s="2" t="s">
+      <c r="J85" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="J85" s="2" t="s">
+      <c r="K85" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="K85" s="2" t="s">
+      <c r="L85" s="2" t="s">
         <v>373</v>
-      </c>
-      <c r="L85" s="2" t="s">
-        <v>374</v>
       </c>
       <c r="M85" s="4" t="s">
         <v>357</v>
@@ -8754,7 +8754,7 @@
         <v>174</v>
       </c>
       <c r="Q85" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="R85" s="2">
         <v>12</v>
@@ -8769,7 +8769,7 @@
         <v>64</v>
       </c>
       <c r="W85" s="7" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="X85" s="5" t="s">
         <v>10</v>
@@ -8778,45 +8778,45 @@
         <v>351</v>
       </c>
       <c r="AA85" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="86" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B86" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="D86" s="2" t="s">
         <v>400</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="D86" s="2" t="s">
-        <v>401</v>
       </c>
       <c r="E86" s="2">
         <v>40</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H86" s="2" t="s">
+        <v>691</v>
+      </c>
+      <c r="I86" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="I86" s="2" t="s">
+      <c r="J86" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="J86" s="2" t="s">
+      <c r="K86" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="K86" s="2" t="s">
+      <c r="L86" s="2" t="s">
         <v>373</v>
-      </c>
-      <c r="L86" s="2" t="s">
-        <v>374</v>
       </c>
       <c r="M86" s="4" t="s">
         <v>357</v>
@@ -8831,7 +8831,7 @@
         <v>174</v>
       </c>
       <c r="Q86" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="R86" s="2">
         <v>12</v>
@@ -8846,7 +8846,7 @@
         <v>64</v>
       </c>
       <c r="W86" s="7" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="X86" s="5" t="s">
         <v>10</v>
@@ -8855,48 +8855,48 @@
         <v>351</v>
       </c>
       <c r="AA86" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="87" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C87" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="D87" s="2" t="s">
         <v>406</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>409</v>
-      </c>
-      <c r="D87" s="2" t="s">
-        <v>407</v>
       </c>
       <c r="E87" s="2">
         <v>16</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="H87" s="7" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="I87" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="J87" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="J87" s="2" t="s">
+      <c r="K87" s="2" t="s">
         <v>419</v>
-      </c>
-      <c r="K87" s="2" t="s">
-        <v>420</v>
       </c>
       <c r="L87" s="2" t="s">
         <v>14</v>
       </c>
       <c r="M87" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="N87" s="5" t="s">
         <v>363</v>
@@ -8905,7 +8905,7 @@
         <v>12</v>
       </c>
       <c r="P87" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="Q87" s="2">
         <v>57000</v>
@@ -8923,7 +8923,7 @@
         <v>301</v>
       </c>
       <c r="W87" s="4" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="X87" s="5" t="s">
         <v>10</v>
@@ -8932,51 +8932,51 @@
         <v>351</v>
       </c>
       <c r="Z87" s="2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="AA87" s="7" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="88" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="C88" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="D88" s="2" t="s">
         <v>412</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>415</v>
-      </c>
-      <c r="D88" s="2" t="s">
-        <v>413</v>
       </c>
       <c r="E88" s="2">
         <v>23</v>
       </c>
       <c r="F88" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="G88" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="G88" s="2" t="s">
+      <c r="H88" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="I88" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="H88" s="7" t="s">
-        <v>404</v>
-      </c>
-      <c r="I88" s="2" t="s">
+      <c r="J88" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="J88" s="2" t="s">
+      <c r="K88" s="2" t="s">
         <v>419</v>
-      </c>
-      <c r="K88" s="2" t="s">
-        <v>420</v>
       </c>
       <c r="L88" s="2" t="s">
         <v>14</v>
       </c>
       <c r="M88" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="N88" s="5" t="s">
         <v>363</v>
@@ -8985,7 +8985,7 @@
         <v>12</v>
       </c>
       <c r="P88" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="Q88" s="2">
         <v>57000</v>
@@ -9003,7 +9003,7 @@
         <v>301</v>
       </c>
       <c r="W88" s="4" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="X88" s="5" t="s">
         <v>10</v>
@@ -9012,39 +9012,39 @@
         <v>351</v>
       </c>
       <c r="Z88" s="2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="AA88" s="7" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="89" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="C89" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="D89" s="2" t="s">
         <v>429</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="D89" s="2" t="s">
-        <v>430</v>
       </c>
       <c r="E89" s="2">
         <v>9</v>
       </c>
       <c r="F89" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="G89" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="G89" s="2" t="s">
-        <v>432</v>
-      </c>
       <c r="H89" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="I89" s="2" t="s">
         <v>425</v>
-      </c>
-      <c r="I89" s="2" t="s">
-        <v>426</v>
       </c>
       <c r="J89" s="2" t="s">
         <v>213</v>
@@ -9056,7 +9056,7 @@
         <v>37</v>
       </c>
       <c r="M89" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="N89" s="4" t="s">
         <v>368</v>
@@ -9083,7 +9083,7 @@
         <v>245</v>
       </c>
       <c r="W89" s="7" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="X89" s="5" t="s">
         <v>10</v>
@@ -9092,39 +9092,39 @@
         <v>351</v>
       </c>
       <c r="Z89" s="2" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="AA89" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="90" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C90" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="D90" s="2" t="s">
         <v>436</v>
-      </c>
-      <c r="D90" s="2" t="s">
-        <v>437</v>
       </c>
       <c r="E90" s="2">
         <v>13</v>
       </c>
       <c r="F90" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="G90" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="G90" s="2" t="s">
-        <v>439</v>
-      </c>
       <c r="H90" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="I90" s="2" t="s">
         <v>425</v>
-      </c>
-      <c r="I90" s="2" t="s">
-        <v>426</v>
       </c>
       <c r="J90" s="2" t="s">
         <v>213</v>
@@ -9136,7 +9136,7 @@
         <v>37</v>
       </c>
       <c r="M90" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="N90" s="4" t="s">
         <v>368</v>
@@ -9163,7 +9163,7 @@
         <v>245</v>
       </c>
       <c r="W90" s="7" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="X90" s="5" t="s">
         <v>10</v>
@@ -9172,39 +9172,39 @@
         <v>351</v>
       </c>
       <c r="Z90" s="2" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="AA90" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="91" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="C91" s="2" t="s">
         <v>444</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="D91" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>445</v>
-      </c>
-      <c r="D91" s="2" t="s">
-        <v>443</v>
       </c>
       <c r="E91" s="2">
         <v>17</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="G91" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H91" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="I91" s="2" t="s">
         <v>425</v>
-      </c>
-      <c r="I91" s="2" t="s">
-        <v>426</v>
       </c>
       <c r="J91" s="2" t="s">
         <v>213</v>
@@ -9216,7 +9216,7 @@
         <v>37</v>
       </c>
       <c r="M91" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="N91" s="4" t="s">
         <v>368</v>
@@ -9243,7 +9243,7 @@
         <v>245</v>
       </c>
       <c r="W91" s="7" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="X91" s="5" t="s">
         <v>10</v>
@@ -9252,36 +9252,36 @@
         <v>351</v>
       </c>
       <c r="Z91" s="2" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="AA91" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="92" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E92" s="2">
         <v>18</v>
       </c>
       <c r="F92" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="G92" s="2" t="s">
         <v>485</v>
       </c>
-      <c r="G92" s="2" t="s">
-        <v>486</v>
-      </c>
       <c r="H92" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="I92" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="I92" s="2" t="s">
+      <c r="J92" s="2" t="s">
         <v>480</v>
-      </c>
-      <c r="J92" s="2" t="s">
-        <v>481</v>
       </c>
       <c r="K92" s="2" t="s">
         <v>60</v>
@@ -9299,7 +9299,7 @@
         <v>12</v>
       </c>
       <c r="P92" s="2" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="Q92" s="2">
         <v>1000</v>
@@ -9317,7 +9317,7 @@
         <v>64</v>
       </c>
       <c r="W92" s="4" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="X92" s="5" t="s">
         <v>10</v>
@@ -9326,36 +9326,36 @@
         <v>351</v>
       </c>
       <c r="Z92" s="7" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="AA92" s="2" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="93" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E93" s="2">
         <v>13</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H93" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="I93" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="I93" s="2" t="s">
+      <c r="J93" s="2" t="s">
         <v>480</v>
-      </c>
-      <c r="J93" s="2" t="s">
-        <v>481</v>
       </c>
       <c r="K93" s="2" t="s">
         <v>60</v>
@@ -9373,7 +9373,7 @@
         <v>12</v>
       </c>
       <c r="P93" s="2" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="Q93" s="2">
         <v>1000</v>
@@ -9391,7 +9391,7 @@
         <v>64</v>
       </c>
       <c r="W93" s="4" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="X93" s="5" t="s">
         <v>10</v>
@@ -9400,45 +9400,45 @@
         <v>350</v>
       </c>
       <c r="Z93" s="2" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="AA93" s="2" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="94" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="C94" s="2" t="s">
         <v>539</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="D94" s="2" t="s">
         <v>537</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>540</v>
-      </c>
-      <c r="D94" s="2" t="s">
-        <v>538</v>
       </c>
       <c r="E94" s="2">
         <v>4</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H94" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="I94" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="I94" s="2" t="s">
+      <c r="J94" s="2" t="s">
         <v>533</v>
       </c>
-      <c r="J94" s="2" t="s">
+      <c r="K94" s="2" t="s">
         <v>534</v>
-      </c>
-      <c r="K94" s="2" t="s">
-        <v>535</v>
       </c>
       <c r="L94" s="2" t="s">
         <v>14</v>
@@ -9471,7 +9471,7 @@
         <v>64</v>
       </c>
       <c r="W94" s="4" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="X94" s="5" t="s">
         <v>10</v>
@@ -9480,45 +9480,45 @@
         <v>351</v>
       </c>
       <c r="Z94" s="7" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="AA94" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="95" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B95" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="D95" s="2" t="s">
         <v>543</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>545</v>
-      </c>
-      <c r="D95" s="2" t="s">
-        <v>544</v>
       </c>
       <c r="E95" s="2">
         <v>8</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="H95" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="I95" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="I95" s="2" t="s">
+      <c r="J95" s="2" t="s">
         <v>533</v>
       </c>
-      <c r="J95" s="2" t="s">
+      <c r="K95" s="2" t="s">
         <v>534</v>
-      </c>
-      <c r="K95" s="2" t="s">
-        <v>535</v>
       </c>
       <c r="L95" s="2" t="s">
         <v>14</v>
@@ -9551,7 +9551,7 @@
         <v>64</v>
       </c>
       <c r="W95" s="4" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="X95" s="5" t="s">
         <v>10</v>
@@ -9560,45 +9560,45 @@
         <v>350</v>
       </c>
       <c r="Z95" s="7" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="AA95" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="96" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="C96" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="B96" s="2" t="s">
-        <v>507</v>
-      </c>
-      <c r="C96" s="2" t="s">
+      <c r="D96" s="2" t="s">
         <v>550</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>551</v>
       </c>
       <c r="E96" s="2">
         <v>12</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="H96" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="I96" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="I96" s="2" t="s">
+      <c r="J96" s="2" t="s">
         <v>533</v>
       </c>
-      <c r="J96" s="2" t="s">
+      <c r="K96" s="2" t="s">
         <v>534</v>
-      </c>
-      <c r="K96" s="2" t="s">
-        <v>535</v>
       </c>
       <c r="L96" s="2" t="s">
         <v>14</v>
@@ -9631,7 +9631,7 @@
         <v>64</v>
       </c>
       <c r="W96" s="4" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="X96" s="5" t="s">
         <v>10</v>
@@ -9640,45 +9640,45 @@
         <v>350</v>
       </c>
       <c r="Z96" s="7" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="AA96" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="97" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="C97" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="D97" s="2" t="s">
         <v>554</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>557</v>
-      </c>
-      <c r="D97" s="2" t="s">
-        <v>555</v>
       </c>
       <c r="E97" s="2">
         <v>16</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="G97" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="H97" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="I97" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="I97" s="2" t="s">
+      <c r="J97" s="2" t="s">
         <v>533</v>
       </c>
-      <c r="J97" s="2" t="s">
+      <c r="K97" s="2" t="s">
         <v>534</v>
-      </c>
-      <c r="K97" s="2" t="s">
-        <v>535</v>
       </c>
       <c r="L97" s="2" t="s">
         <v>14</v>
@@ -9711,7 +9711,7 @@
         <v>64</v>
       </c>
       <c r="W97" s="4" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="X97" s="5" t="s">
         <v>10</v>
@@ -9720,45 +9720,45 @@
         <v>351</v>
       </c>
       <c r="Z97" s="7" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="AA97" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="98" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="C98" s="2" t="s">
         <v>561</v>
       </c>
-      <c r="B98" s="2" t="s">
-        <v>560</v>
-      </c>
-      <c r="C98" s="2" t="s">
+      <c r="D98" s="2" t="s">
         <v>562</v>
-      </c>
-      <c r="D98" s="2" t="s">
-        <v>563</v>
       </c>
       <c r="E98" s="2">
         <v>20</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="G98" s="2" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="H98" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="I98" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="I98" s="2" t="s">
+      <c r="J98" s="2" t="s">
         <v>533</v>
       </c>
-      <c r="J98" s="2" t="s">
+      <c r="K98" s="2" t="s">
         <v>534</v>
-      </c>
-      <c r="K98" s="2" t="s">
-        <v>535</v>
       </c>
       <c r="L98" s="2" t="s">
         <v>14</v>
@@ -9791,7 +9791,7 @@
         <v>64</v>
       </c>
       <c r="W98" s="4" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="X98" s="5" t="s">
         <v>10</v>
@@ -9800,45 +9800,45 @@
         <v>351</v>
       </c>
       <c r="Z98" s="7" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="AA98" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="99" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="C99" s="2" t="s">
         <v>567</v>
       </c>
-      <c r="B99" s="2" t="s">
-        <v>566</v>
-      </c>
-      <c r="C99" s="2" t="s">
+      <c r="D99" s="2" t="s">
         <v>568</v>
-      </c>
-      <c r="D99" s="2" t="s">
-        <v>569</v>
       </c>
       <c r="E99" s="2">
         <v>24</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="G99" s="2" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H99" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="I99" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="I99" s="2" t="s">
+      <c r="J99" s="2" t="s">
         <v>533</v>
       </c>
-      <c r="J99" s="2" t="s">
+      <c r="K99" s="2" t="s">
         <v>534</v>
-      </c>
-      <c r="K99" s="2" t="s">
-        <v>535</v>
       </c>
       <c r="L99" s="2" t="s">
         <v>14</v>
@@ -9871,7 +9871,7 @@
         <v>64</v>
       </c>
       <c r="W99" s="4" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="X99" s="5" t="s">
         <v>10</v>
@@ -9880,42 +9880,42 @@
         <v>351</v>
       </c>
       <c r="Z99" s="7" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="AA99" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="100" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="C100" s="2" t="s">
         <v>589</v>
       </c>
-      <c r="B100" s="2" t="s">
-        <v>588</v>
-      </c>
-      <c r="C100" s="2" t="s">
+      <c r="D100" s="2" t="s">
         <v>590</v>
-      </c>
-      <c r="D100" s="2" t="s">
-        <v>591</v>
       </c>
       <c r="E100" s="2">
         <v>20</v>
       </c>
       <c r="F100" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="G100" s="2" t="s">
         <v>592</v>
       </c>
-      <c r="G100" s="2" t="s">
-        <v>593</v>
-      </c>
       <c r="H100" s="2" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I100" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="J100" s="2" t="s">
         <v>600</v>
-      </c>
-      <c r="J100" s="2" t="s">
-        <v>601</v>
       </c>
       <c r="K100" s="2" t="s">
         <v>330</v>
@@ -9951,7 +9951,7 @@
         <v>64</v>
       </c>
       <c r="W100" s="12" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="X100" s="5" t="s">
         <v>10</v>
@@ -9960,42 +9960,42 @@
         <v>351</v>
       </c>
       <c r="Z100" s="2" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="AA100" s="2" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="101" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="C101" s="2" t="s">
         <v>595</v>
       </c>
-      <c r="B101" s="2" t="s">
-        <v>594</v>
-      </c>
-      <c r="C101" s="2" t="s">
+      <c r="D101" s="2" t="s">
         <v>596</v>
-      </c>
-      <c r="D101" s="2" t="s">
-        <v>597</v>
       </c>
       <c r="E101" s="2">
         <v>27</v>
       </c>
       <c r="F101" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="G101" s="2" t="s">
         <v>598</v>
       </c>
-      <c r="G101" s="2" t="s">
+      <c r="H101" s="2" t="s">
+        <v>586</v>
+      </c>
+      <c r="I101" s="2" t="s">
         <v>599</v>
       </c>
-      <c r="H101" s="2" t="s">
-        <v>587</v>
-      </c>
-      <c r="I101" s="2" t="s">
+      <c r="J101" s="2" t="s">
         <v>600</v>
-      </c>
-      <c r="J101" s="2" t="s">
-        <v>601</v>
       </c>
       <c r="K101" s="2" t="s">
         <v>330</v>
@@ -10031,7 +10031,7 @@
         <v>64</v>
       </c>
       <c r="W101" s="12" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="X101" s="5" t="s">
         <v>10</v>
@@ -10040,45 +10040,45 @@
         <v>351</v>
       </c>
       <c r="Z101" s="2" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="AA101" s="2" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="102" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="C102" s="2" t="s">
         <v>502</v>
       </c>
-      <c r="B102" s="2" t="s">
-        <v>501</v>
-      </c>
-      <c r="C102" s="2" t="s">
+      <c r="D102" s="2" t="s">
         <v>503</v>
-      </c>
-      <c r="D102" s="2" t="s">
-        <v>504</v>
       </c>
       <c r="E102" s="2">
         <v>10</v>
       </c>
       <c r="F102" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="G102" s="2" t="s">
         <v>505</v>
       </c>
-      <c r="G102" s="2" t="s">
-        <v>506</v>
-      </c>
       <c r="H102" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="I102" s="2" t="s">
         <v>519</v>
-      </c>
-      <c r="I102" s="2" t="s">
-        <v>520</v>
       </c>
       <c r="J102" s="2" t="s">
         <v>150</v>
       </c>
       <c r="K102" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="L102" s="2" t="s">
         <v>36</v>
@@ -10120,45 +10120,45 @@
         <v>351</v>
       </c>
       <c r="Z102" s="2" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="AA102" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="103" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="C103" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="B103" s="2" t="s">
+      <c r="D103" s="2" t="s">
         <v>507</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>510</v>
-      </c>
-      <c r="D103" s="2" t="s">
-        <v>508</v>
       </c>
       <c r="E103" s="2">
         <v>12</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="G103" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="H103" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="I103" s="2" t="s">
         <v>519</v>
-      </c>
-      <c r="I103" s="2" t="s">
-        <v>520</v>
       </c>
       <c r="J103" s="2" t="s">
         <v>150</v>
       </c>
       <c r="K103" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="L103" s="2" t="s">
         <v>36</v>
@@ -10200,45 +10200,45 @@
         <v>350</v>
       </c>
       <c r="Z103" s="2" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="AA103" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="104" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="C104" s="2" t="s">
         <v>514</v>
       </c>
-      <c r="B104" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="C104" s="2" t="s">
+      <c r="D104" s="2" t="s">
         <v>515</v>
-      </c>
-      <c r="D104" s="2" t="s">
-        <v>516</v>
       </c>
       <c r="E104" s="2">
         <v>15</v>
       </c>
       <c r="F104" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="G104" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="H104" s="2" t="s">
         <v>518</v>
       </c>
-      <c r="G104" s="2" t="s">
-        <v>517</v>
-      </c>
-      <c r="H104" s="2" t="s">
+      <c r="I104" s="2" t="s">
         <v>519</v>
-      </c>
-      <c r="I104" s="2" t="s">
-        <v>520</v>
       </c>
       <c r="J104" s="2" t="s">
         <v>150</v>
       </c>
       <c r="K104" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="L104" s="2" t="s">
         <v>36</v>
@@ -10280,33 +10280,33 @@
         <v>351</v>
       </c>
       <c r="Z104" s="2" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="AA104" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="105" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E105" s="2">
         <v>18</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="G105" s="2">
         <v>1</v>
       </c>
       <c r="H105" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="I105" s="2" t="s">
         <v>469</v>
-      </c>
-      <c r="I105" s="2" t="s">
-        <v>470</v>
       </c>
       <c r="J105" s="2" t="s">
         <v>150</v>
@@ -10318,7 +10318,7 @@
         <v>37</v>
       </c>
       <c r="M105" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="N105" s="4" t="s">
         <v>368</v>
@@ -10342,10 +10342,10 @@
         <v>9</v>
       </c>
       <c r="U105" s="4" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="W105" s="4" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="X105" s="2" t="s">
         <v>21</v>
@@ -10354,33 +10354,33 @@
         <v>351</v>
       </c>
       <c r="Z105" s="2" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="AA105" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="106" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="E106" s="2">
         <v>12</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="G106" s="2">
         <v>1</v>
       </c>
       <c r="H106" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="I106" s="2" t="s">
         <v>469</v>
-      </c>
-      <c r="I106" s="2" t="s">
-        <v>470</v>
       </c>
       <c r="J106" s="2" t="s">
         <v>150</v>
@@ -10392,7 +10392,7 @@
         <v>37</v>
       </c>
       <c r="M106" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="N106" s="4" t="s">
         <v>368</v>
@@ -10416,10 +10416,10 @@
         <v>9</v>
       </c>
       <c r="U106" s="4" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="W106" s="4" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="X106" s="2" t="s">
         <v>21</v>
@@ -10428,33 +10428,33 @@
         <v>351</v>
       </c>
       <c r="Z106" s="2" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="AA106" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="107" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="E107" s="2">
         <v>6</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="G107" s="2">
         <v>1</v>
       </c>
       <c r="H107" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="I107" s="2" t="s">
         <v>469</v>
-      </c>
-      <c r="I107" s="2" t="s">
-        <v>470</v>
       </c>
       <c r="J107" s="2" t="s">
         <v>150</v>
@@ -10466,7 +10466,7 @@
         <v>37</v>
       </c>
       <c r="M107" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="N107" s="4" t="s">
         <v>368</v>
@@ -10490,10 +10490,10 @@
         <v>9</v>
       </c>
       <c r="U107" s="4" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="W107" s="4" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="X107" s="2" t="s">
         <v>21</v>
@@ -10502,10 +10502,10 @@
         <v>351</v>
       </c>
       <c r="Z107" s="2" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="AA107" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="108" spans="1:27" x14ac:dyDescent="0.25">
@@ -10574,7 +10574,7 @@
       </c>
       <c r="V108" s="4"/>
       <c r="W108" s="4" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="X108" s="4" t="s">
         <v>21</v>
@@ -10583,7 +10583,7 @@
         <v>351</v>
       </c>
       <c r="Z108" s="2" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="AA108" s="4" t="s">
         <v>348</v>
@@ -10655,7 +10655,7 @@
       </c>
       <c r="V109" s="4"/>
       <c r="W109" s="4" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="X109" s="4" t="s">
         <v>21</v>
@@ -10664,7 +10664,7 @@
         <v>351</v>
       </c>
       <c r="Z109" s="2" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="AA109" s="4" t="s">
         <v>348</v>
@@ -10672,31 +10672,31 @@
     </row>
     <row r="110" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
+        <v>653</v>
+      </c>
+      <c r="B110" s="2" t="s">
         <v>654</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>655</v>
       </c>
       <c r="E110" s="2">
         <v>17</v>
       </c>
       <c r="F110" t="s">
+        <v>682</v>
+      </c>
+      <c r="G110" t="s">
         <v>683</v>
       </c>
-      <c r="G110" t="s">
-        <v>684</v>
-      </c>
       <c r="H110" s="7" t="s">
+        <v>645</v>
+      </c>
+      <c r="I110" s="7" t="s">
         <v>646</v>
       </c>
-      <c r="I110" s="7" t="s">
+      <c r="J110" s="7" t="s">
         <v>647</v>
       </c>
-      <c r="J110" s="7" t="s">
+      <c r="K110" s="7" t="s">
         <v>648</v>
-      </c>
-      <c r="K110" s="7" t="s">
-        <v>649</v>
       </c>
       <c r="L110" s="7" t="s">
         <v>14</v>
@@ -10705,13 +10705,13 @@
         <v>356</v>
       </c>
       <c r="N110" s="7" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="O110" s="7" t="s">
         <v>62</v>
       </c>
       <c r="P110" s="7" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="Q110" s="7">
         <v>15000</v>
@@ -10726,11 +10726,11 @@
         <v>64</v>
       </c>
       <c r="U110" s="7" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="V110" s="7"/>
       <c r="W110" s="2" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="X110" s="4" t="s">
         <v>21</v>
@@ -10739,36 +10739,36 @@
         <v>351</v>
       </c>
       <c r="AA110" s="7" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="111" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="B111" s="2" t="s">
         <v>656</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>657</v>
       </c>
       <c r="E111" s="2">
         <v>21</v>
       </c>
       <c r="F111" t="s">
+        <v>684</v>
+      </c>
+      <c r="G111" t="s">
         <v>685</v>
       </c>
-      <c r="G111" t="s">
-        <v>686</v>
-      </c>
       <c r="H111" s="7" t="s">
+        <v>645</v>
+      </c>
+      <c r="I111" s="7" t="s">
         <v>646</v>
       </c>
-      <c r="I111" s="7" t="s">
+      <c r="J111" s="7" t="s">
         <v>647</v>
       </c>
-      <c r="J111" s="7" t="s">
+      <c r="K111" s="7" t="s">
         <v>648</v>
-      </c>
-      <c r="K111" s="7" t="s">
-        <v>649</v>
       </c>
       <c r="L111" s="7" t="s">
         <v>14</v>
@@ -10777,13 +10777,13 @@
         <v>356</v>
       </c>
       <c r="N111" s="7" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="O111" s="7" t="s">
         <v>62</v>
       </c>
       <c r="P111" s="7" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="Q111" s="7">
         <v>15000</v>
@@ -10798,11 +10798,11 @@
         <v>64</v>
       </c>
       <c r="U111" s="7" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="V111" s="7"/>
       <c r="W111" s="2" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="X111" s="4" t="s">
         <v>21</v>
@@ -10811,15 +10811,15 @@
         <v>351</v>
       </c>
       <c r="AA111" s="7" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="112" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
+        <v>657</v>
+      </c>
+      <c r="B112" s="2" t="s">
         <v>658</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>659</v>
       </c>
       <c r="E112" s="2">
         <v>25</v>
@@ -10828,19 +10828,19 @@
         <v>25</v>
       </c>
       <c r="G112" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="H112" s="7" t="s">
+        <v>645</v>
+      </c>
+      <c r="I112" s="7" t="s">
         <v>646</v>
       </c>
-      <c r="I112" s="7" t="s">
+      <c r="J112" s="7" t="s">
         <v>647</v>
       </c>
-      <c r="J112" s="7" t="s">
+      <c r="K112" s="7" t="s">
         <v>648</v>
-      </c>
-      <c r="K112" s="7" t="s">
-        <v>649</v>
       </c>
       <c r="L112" s="7" t="s">
         <v>14</v>
@@ -10849,13 +10849,13 @@
         <v>356</v>
       </c>
       <c r="N112" s="7" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="O112" s="7" t="s">
         <v>62</v>
       </c>
       <c r="P112" s="7" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="Q112" s="7">
         <v>15000</v>
@@ -10870,11 +10870,11 @@
         <v>64</v>
       </c>
       <c r="U112" s="7" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="V112" s="7"/>
       <c r="W112" s="2" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="X112" s="4" t="s">
         <v>21</v>
@@ -10883,36 +10883,36 @@
         <v>351</v>
       </c>
       <c r="AA112" s="7" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="113" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="B113" s="2" t="s">
         <v>660</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>661</v>
       </c>
       <c r="E113" s="2">
         <v>30</v>
       </c>
       <c r="F113" t="s">
+        <v>687</v>
+      </c>
+      <c r="G113" t="s">
         <v>688</v>
       </c>
-      <c r="G113" t="s">
-        <v>689</v>
-      </c>
       <c r="H113" s="7" t="s">
+        <v>645</v>
+      </c>
+      <c r="I113" s="7" t="s">
         <v>646</v>
       </c>
-      <c r="I113" s="7" t="s">
+      <c r="J113" s="7" t="s">
         <v>647</v>
       </c>
-      <c r="J113" s="7" t="s">
+      <c r="K113" s="7" t="s">
         <v>648</v>
-      </c>
-      <c r="K113" s="7" t="s">
-        <v>649</v>
       </c>
       <c r="L113" s="7" t="s">
         <v>14</v>
@@ -10921,13 +10921,13 @@
         <v>356</v>
       </c>
       <c r="N113" s="7" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="O113" s="7" t="s">
         <v>62</v>
       </c>
       <c r="P113" s="7" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="Q113" s="7">
         <v>15000</v>
@@ -10942,11 +10942,11 @@
         <v>64</v>
       </c>
       <c r="U113" s="7" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="V113" s="7"/>
       <c r="W113" s="2" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="X113" s="4" t="s">
         <v>21</v>
@@ -10955,36 +10955,36 @@
         <v>351</v>
       </c>
       <c r="AA113" s="7" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="114" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="B114" s="2" t="s">
         <v>662</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>663</v>
       </c>
       <c r="E114" s="2">
         <v>35</v>
       </c>
       <c r="F114" t="s">
+        <v>689</v>
+      </c>
+      <c r="G114" t="s">
         <v>690</v>
       </c>
-      <c r="G114" t="s">
-        <v>691</v>
-      </c>
       <c r="H114" s="7" t="s">
+        <v>645</v>
+      </c>
+      <c r="I114" s="7" t="s">
         <v>646</v>
       </c>
-      <c r="I114" s="7" t="s">
+      <c r="J114" s="7" t="s">
         <v>647</v>
       </c>
-      <c r="J114" s="7" t="s">
+      <c r="K114" s="7" t="s">
         <v>648</v>
-      </c>
-      <c r="K114" s="7" t="s">
-        <v>649</v>
       </c>
       <c r="L114" s="7" t="s">
         <v>14</v>
@@ -10993,13 +10993,13 @@
         <v>356</v>
       </c>
       <c r="N114" s="7" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="O114" s="7" t="s">
         <v>62</v>
       </c>
       <c r="P114" s="7" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="Q114" s="7">
         <v>15000</v>
@@ -11014,11 +11014,11 @@
         <v>64</v>
       </c>
       <c r="U114" s="7" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="V114" s="7"/>
       <c r="W114" s="2" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="X114" s="4" t="s">
         <v>21</v>
@@ -11027,7 +11027,7 @@
         <v>351</v>
       </c>
       <c r="AA114" s="7" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
   </sheetData>

</xml_diff>